<commit_message>
TT-2466d update sample spreadsheets
</commit_message>
<xml_diff>
--- a/help/Luke4-5-flat.xlsx
+++ b/help/Luke4-5-flat.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Trihus\Desktop\TypeScript Samples\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Trihus\git\transcriber\help\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,12 +19,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
   <si>
     <t>Set #</t>
-  </si>
-  <si>
-    <t>Passage</t>
   </si>
   <si>
     <t>Breaks</t>
@@ -882,139 +879,118 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD8"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="47" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
       </c>
       <c r="D2" t="s">
         <v>6</v>
       </c>
-      <c r="E2" t="s">
-        <v>7</v>
-      </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" t="s">
         <v>9</v>
       </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" t="s">
-        <v>10</v>
-      </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
       </c>
       <c r="D4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" t="s">
         <v>13</v>
       </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" t="s">
-        <v>14</v>
-      </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" t="s">
         <v>15</v>
       </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-      <c r="D6" t="s">
-        <v>6</v>
-      </c>
-      <c r="E6" t="s">
-        <v>16</v>
-      </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" t="s">
         <v>17</v>
-      </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-      <c r="D7" t="s">
-        <v>6</v>
-      </c>
-      <c r="E7" t="s">
-        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>